<commit_message>
added user manual and testdoc
</commit_message>
<xml_diff>
--- a/test_doc.xlsx
+++ b/test_doc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289">
   <si>
     <t>No.</t>
   </si>
@@ -656,6 +656,51 @@
   </si>
   <si>
     <t>The cancel button should generate go back link on clicking</t>
+  </si>
+  <si>
+    <t>Admin Home Page</t>
+  </si>
+  <si>
+    <t>Background should display the Log out  button or link</t>
+  </si>
+  <si>
+    <t>Add New User Link</t>
+  </si>
+  <si>
+    <t>Link should be clickable</t>
+  </si>
+  <si>
+    <t>Link should redirects to Sign UP page</t>
+  </si>
+  <si>
+    <t>Remove User Link</t>
+  </si>
+  <si>
+    <t>Link should Redirects to Remove user page</t>
+  </si>
+  <si>
+    <t>Add New Resarch Paper Link</t>
+  </si>
+  <si>
+    <t>Link should redirects to Add New resaerch Paper page</t>
+  </si>
+  <si>
+    <t>Update Research Paper Link</t>
+  </si>
+  <si>
+    <t>Link should redirects to Update Research Paper page</t>
+  </si>
+  <si>
+    <t>Update user Detail Link</t>
+  </si>
+  <si>
+    <t>Link should Redirects to Update User Details Page</t>
+  </si>
+  <si>
+    <t>View Research Paper Link</t>
+  </si>
+  <si>
+    <t>Link should redirects to View Research Paper page</t>
   </si>
   <si>
     <t>SIGN UP page</t>
@@ -846,22 +891,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1006,40 +1046,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,7 +1096,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1070,40 +1110,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1425,11 +1435,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -1453,12 +1463,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AA300"/>
+  <dimension ref="A1:AA321"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E303" sqref="E303"/>
+      <selection pane="bottomLeft" activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4490,24 +4500,24 @@
       </c>
     </row>
     <row r="190" spans="1:6">
-      <c r="A190" s="21"/>
-      <c r="B190" s="22"/>
-      <c r="C190" s="22"/>
-      <c r="D190" s="23"/>
-      <c r="E190" s="24"/>
-      <c r="F190" s="25"/>
+      <c r="A190" s="11"/>
+      <c r="B190" s="12"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="12"/>
+      <c r="F190" s="19"/>
     </row>
     <row r="191" spans="1:6">
-      <c r="A191" s="26">
+      <c r="A191" s="11">
         <v>7</v>
       </c>
-      <c r="B191" s="27" t="s">
+      <c r="B191" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="C191" s="28">
+      <c r="C191" s="12">
         <v>1</v>
       </c>
-      <c r="D191" s="29" t="s">
+      <c r="D191" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E191" s="12" t="s">
@@ -4518,12 +4528,12 @@
       </c>
     </row>
     <row r="192" spans="1:6">
-      <c r="A192" s="21"/>
-      <c r="B192" s="22"/>
-      <c r="C192" s="22">
+      <c r="A192" s="11"/>
+      <c r="B192" s="12"/>
+      <c r="C192" s="12">
         <v>2</v>
       </c>
-      <c r="D192" s="30" t="s">
+      <c r="D192" s="13" t="s">
         <v>6</v>
       </c>
       <c r="E192" s="12" t="s">
@@ -4534,12 +4544,12 @@
       </c>
     </row>
     <row r="193" spans="1:6">
-      <c r="A193" s="21"/>
-      <c r="B193" s="22"/>
-      <c r="C193" s="22">
+      <c r="A193" s="11"/>
+      <c r="B193" s="12"/>
+      <c r="C193" s="12">
         <v>3</v>
       </c>
-      <c r="D193" s="30" t="s">
+      <c r="D193" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E193" s="12" t="s">
@@ -4550,12 +4560,12 @@
       </c>
     </row>
     <row r="194" spans="1:6">
-      <c r="A194" s="21"/>
-      <c r="B194" s="22"/>
-      <c r="C194" s="22">
+      <c r="A194" s="11"/>
+      <c r="B194" s="12"/>
+      <c r="C194" s="12">
         <v>4</v>
       </c>
-      <c r="D194" s="30" t="s">
+      <c r="D194" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E194" s="15" t="s">
@@ -4566,12 +4576,12 @@
       </c>
     </row>
     <row r="195" spans="1:6">
-      <c r="A195" s="21"/>
-      <c r="B195" s="22"/>
-      <c r="C195" s="22">
+      <c r="A195" s="11"/>
+      <c r="B195" s="12"/>
+      <c r="C195" s="12">
         <v>5</v>
       </c>
-      <c r="D195" s="30" t="s">
+      <c r="D195" s="13" t="s">
         <v>106</v>
       </c>
       <c r="E195" s="15" t="s">
@@ -4582,12 +4592,12 @@
       </c>
     </row>
     <row r="196" spans="1:6">
-      <c r="A196" s="21"/>
-      <c r="B196" s="22"/>
-      <c r="C196" s="22">
+      <c r="A196" s="11"/>
+      <c r="B196" s="12"/>
+      <c r="C196" s="12">
         <v>6</v>
       </c>
-      <c r="D196" s="30" t="s">
+      <c r="D196" s="13" t="s">
         <v>106</v>
       </c>
       <c r="E196" s="15" t="s">
@@ -4598,15 +4608,15 @@
       </c>
     </row>
     <row r="197" spans="1:6">
-      <c r="A197" s="21"/>
-      <c r="B197" s="22"/>
-      <c r="C197" s="22">
+      <c r="A197" s="11"/>
+      <c r="B197" s="12"/>
+      <c r="C197" s="12">
         <v>7</v>
       </c>
-      <c r="D197" s="30" t="s">
+      <c r="D197" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E197" s="31" t="s">
+      <c r="E197" s="15" t="s">
         <v>194</v>
       </c>
       <c r="F197" s="14" t="s">
@@ -4614,15 +4624,15 @@
       </c>
     </row>
     <row r="198" spans="1:6">
-      <c r="A198" s="21"/>
-      <c r="B198" s="22"/>
-      <c r="C198" s="22">
-        <v>8</v>
-      </c>
-      <c r="D198" s="30" t="s">
+      <c r="A198" s="11"/>
+      <c r="B198" s="12"/>
+      <c r="C198" s="12">
+        <v>8</v>
+      </c>
+      <c r="D198" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E198" s="22" t="s">
+      <c r="E198" s="12" t="s">
         <v>195</v>
       </c>
       <c r="F198" s="14" t="s">
@@ -4630,15 +4640,15 @@
       </c>
     </row>
     <row r="199" spans="1:6">
-      <c r="A199" s="21"/>
-      <c r="B199" s="22"/>
-      <c r="C199" s="22">
+      <c r="A199" s="11"/>
+      <c r="B199" s="12"/>
+      <c r="C199" s="12">
         <v>9</v>
       </c>
-      <c r="D199" s="30" t="s">
+      <c r="D199" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E199" s="22" t="s">
+      <c r="E199" s="12" t="s">
         <v>196</v>
       </c>
       <c r="F199" s="14" t="s">
@@ -4646,15 +4656,15 @@
       </c>
     </row>
     <row r="200" spans="1:6">
-      <c r="A200" s="21"/>
-      <c r="B200" s="22"/>
-      <c r="C200" s="22">
+      <c r="A200" s="11"/>
+      <c r="B200" s="12"/>
+      <c r="C200" s="12">
         <v>10</v>
       </c>
-      <c r="D200" s="30" t="s">
+      <c r="D200" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="E200" s="22" t="s">
+      <c r="E200" s="12" t="s">
         <v>197</v>
       </c>
       <c r="F200" s="14" t="s">
@@ -4662,15 +4672,15 @@
       </c>
     </row>
     <row r="201" spans="1:6">
-      <c r="A201" s="21"/>
-      <c r="B201" s="22"/>
-      <c r="C201" s="22">
+      <c r="A201" s="11"/>
+      <c r="B201" s="12"/>
+      <c r="C201" s="12">
         <v>11</v>
       </c>
-      <c r="D201" s="30" t="s">
+      <c r="D201" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E201" s="22" t="s">
+      <c r="E201" s="12" t="s">
         <v>199</v>
       </c>
       <c r="F201" s="14" t="s">
@@ -4678,15 +4688,15 @@
       </c>
     </row>
     <row r="202" spans="1:6">
-      <c r="A202" s="21"/>
-      <c r="B202" s="22"/>
-      <c r="C202" s="22">
-        <v>12</v>
-      </c>
-      <c r="D202" s="30" t="s">
+      <c r="A202" s="11"/>
+      <c r="B202" s="12"/>
+      <c r="C202" s="12">
+        <v>12</v>
+      </c>
+      <c r="D202" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E202" s="31" t="s">
+      <c r="E202" s="15" t="s">
         <v>200</v>
       </c>
       <c r="F202" s="14" t="s">
@@ -4694,15 +4704,15 @@
       </c>
     </row>
     <row r="203" spans="1:6">
-      <c r="A203" s="21"/>
-      <c r="B203" s="22"/>
-      <c r="C203" s="22">
+      <c r="A203" s="11"/>
+      <c r="B203" s="12"/>
+      <c r="C203" s="12">
         <v>13</v>
       </c>
-      <c r="D203" s="30" t="s">
+      <c r="D203" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E203" s="22" t="s">
+      <c r="E203" s="12" t="s">
         <v>201</v>
       </c>
       <c r="F203" s="14" t="s">
@@ -4710,15 +4720,15 @@
       </c>
     </row>
     <row r="204" spans="1:6">
-      <c r="A204" s="21"/>
-      <c r="B204" s="22"/>
-      <c r="C204" s="22">
+      <c r="A204" s="11"/>
+      <c r="B204" s="12"/>
+      <c r="C204" s="12">
         <v>14</v>
       </c>
-      <c r="D204" s="30" t="s">
+      <c r="D204" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E204" s="22" t="s">
+      <c r="E204" s="12" t="s">
         <v>202</v>
       </c>
       <c r="F204" s="14" t="s">
@@ -4726,15 +4736,15 @@
       </c>
     </row>
     <row r="205" spans="1:6">
-      <c r="A205" s="21"/>
-      <c r="B205" s="22"/>
-      <c r="C205" s="22">
+      <c r="A205" s="11"/>
+      <c r="B205" s="12"/>
+      <c r="C205" s="12">
         <v>15</v>
       </c>
-      <c r="D205" s="30" t="s">
+      <c r="D205" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="E205" s="22" t="s">
+      <c r="E205" s="12" t="s">
         <v>203</v>
       </c>
       <c r="F205" s="14" t="s">
@@ -4742,15 +4752,15 @@
       </c>
     </row>
     <row r="206" spans="1:6">
-      <c r="A206" s="21"/>
-      <c r="B206" s="22"/>
-      <c r="C206" s="22">
+      <c r="A206" s="11"/>
+      <c r="B206" s="12"/>
+      <c r="C206" s="12">
         <v>16</v>
       </c>
-      <c r="D206" s="30" t="s">
+      <c r="D206" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E206" s="22" t="s">
+      <c r="E206" s="12" t="s">
         <v>205</v>
       </c>
       <c r="F206" s="14" t="s">
@@ -4758,15 +4768,15 @@
       </c>
     </row>
     <row r="207" spans="1:6">
-      <c r="A207" s="21"/>
-      <c r="B207" s="22"/>
-      <c r="C207" s="22">
+      <c r="A207" s="11"/>
+      <c r="B207" s="12"/>
+      <c r="C207" s="12">
         <v>17</v>
       </c>
-      <c r="D207" s="30" t="s">
+      <c r="D207" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E207" s="22" t="s">
+      <c r="E207" s="12" t="s">
         <v>206</v>
       </c>
       <c r="F207" s="14" t="s">
@@ -4774,15 +4784,15 @@
       </c>
     </row>
     <row r="208" spans="1:6">
-      <c r="A208" s="21"/>
-      <c r="B208" s="22"/>
-      <c r="C208" s="22">
+      <c r="A208" s="11"/>
+      <c r="B208" s="12"/>
+      <c r="C208" s="12">
         <v>18</v>
       </c>
-      <c r="D208" s="30" t="s">
+      <c r="D208" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E208" s="22" t="s">
+      <c r="E208" s="12" t="s">
         <v>207</v>
       </c>
       <c r="F208" s="14" t="s">
@@ -4790,15 +4800,15 @@
       </c>
     </row>
     <row r="209" spans="1:6">
-      <c r="A209" s="21"/>
-      <c r="B209" s="22"/>
-      <c r="C209" s="22">
+      <c r="A209" s="11"/>
+      <c r="B209" s="12"/>
+      <c r="C209" s="12">
         <v>19</v>
       </c>
-      <c r="D209" s="30" t="s">
+      <c r="D209" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="E209" s="22" t="s">
+      <c r="E209" s="12" t="s">
         <v>209</v>
       </c>
       <c r="F209" s="14" t="s">
@@ -4806,15 +4816,15 @@
       </c>
     </row>
     <row r="210" spans="1:6">
-      <c r="A210" s="21"/>
-      <c r="B210" s="22"/>
-      <c r="C210" s="22">
+      <c r="A210" s="11"/>
+      <c r="B210" s="12"/>
+      <c r="C210" s="12">
         <v>20</v>
       </c>
-      <c r="D210" s="30" t="s">
+      <c r="D210" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="E210" s="22" t="s">
+      <c r="E210" s="12" t="s">
         <v>210</v>
       </c>
       <c r="F210" s="14" t="s">
@@ -4822,15 +4832,15 @@
       </c>
     </row>
     <row r="211" spans="1:6">
-      <c r="A211" s="21"/>
-      <c r="B211" s="22"/>
-      <c r="C211" s="22">
+      <c r="A211" s="11"/>
+      <c r="B211" s="12"/>
+      <c r="C211" s="12">
         <v>21</v>
       </c>
-      <c r="D211" s="30" t="s">
+      <c r="D211" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="E211" s="22" t="s">
+      <c r="E211" s="12" t="s">
         <v>211</v>
       </c>
       <c r="F211" s="14" t="s">
@@ -4838,15 +4848,15 @@
       </c>
     </row>
     <row r="212" spans="1:6">
-      <c r="A212" s="32"/>
-      <c r="B212" s="33"/>
-      <c r="C212" s="33">
+      <c r="A212" s="11"/>
+      <c r="B212" s="12"/>
+      <c r="C212" s="12">
         <v>22</v>
       </c>
-      <c r="D212" s="34" t="s">
+      <c r="D212" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="E212" s="33" t="s">
+      <c r="E212" s="12" t="s">
         <v>212</v>
       </c>
       <c r="F212" s="14" t="s">
@@ -4854,27 +4864,27 @@
       </c>
     </row>
     <row r="213" spans="1:6">
-      <c r="A213" s="21"/>
-      <c r="B213" s="22"/>
-      <c r="C213" s="22"/>
-      <c r="D213" s="22"/>
-      <c r="E213" s="22"/>
-      <c r="F213" s="35"/>
+      <c r="A213" s="11"/>
+      <c r="B213" s="12"/>
+      <c r="C213" s="12"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="12"/>
+      <c r="F213" s="14"/>
     </row>
     <row r="214" spans="1:6">
-      <c r="A214" s="11">
-        <v>8</v>
-      </c>
-      <c r="B214" s="16" t="s">
+      <c r="A214" s="21">
+        <v>8</v>
+      </c>
+      <c r="B214" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="C214" s="12">
+      <c r="C214" s="23">
         <v>1</v>
       </c>
       <c r="D214" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E214" s="12" t="s">
+      <c r="E214" s="23" t="s">
         <v>7</v>
       </c>
       <c r="F214" s="14" t="s">
@@ -4882,15 +4892,15 @@
       </c>
     </row>
     <row r="215" spans="1:6">
-      <c r="A215" s="11"/>
-      <c r="B215" s="12"/>
-      <c r="C215" s="12">
+      <c r="A215" s="21"/>
+      <c r="B215" s="23"/>
+      <c r="C215" s="23">
         <v>2</v>
       </c>
       <c r="D215" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E215" s="12" t="s">
+      <c r="E215" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F215" s="14" t="s">
@@ -4898,15 +4908,15 @@
       </c>
     </row>
     <row r="216" spans="1:6">
-      <c r="A216" s="11"/>
-      <c r="B216" s="12"/>
-      <c r="C216" s="12">
+      <c r="A216" s="21"/>
+      <c r="B216" s="23"/>
+      <c r="C216" s="23">
         <v>3</v>
       </c>
       <c r="D216" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E216" s="12" t="s">
+      <c r="E216" s="23" t="s">
         <v>13</v>
       </c>
       <c r="F216" s="14" t="s">
@@ -4914,15 +4924,15 @@
       </c>
     </row>
     <row r="217" spans="1:6">
-      <c r="A217" s="11"/>
-      <c r="B217" s="12"/>
-      <c r="C217" s="12">
+      <c r="A217" s="21"/>
+      <c r="B217" s="23"/>
+      <c r="C217" s="23">
         <v>4</v>
       </c>
       <c r="D217" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E217" s="12" t="s">
+      <c r="E217" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F217" s="14" t="s">
@@ -4930,15 +4940,15 @@
       </c>
     </row>
     <row r="218" spans="1:6">
-      <c r="A218" s="11"/>
-      <c r="B218" s="12"/>
-      <c r="C218" s="12">
+      <c r="A218" s="21"/>
+      <c r="B218" s="23"/>
+      <c r="C218" s="23">
         <v>5</v>
       </c>
       <c r="D218" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E218" s="12" t="s">
+      <c r="E218" s="23" t="s">
         <v>15</v>
       </c>
       <c r="F218" s="14" t="s">
@@ -4946,15 +4956,15 @@
       </c>
     </row>
     <row r="219" spans="1:6">
-      <c r="A219" s="11"/>
-      <c r="B219" s="12"/>
-      <c r="C219" s="12">
+      <c r="A219" s="21"/>
+      <c r="B219" s="23"/>
+      <c r="C219" s="23">
         <v>6</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E219" s="15" t="s">
+      <c r="E219" s="24" t="s">
         <v>16</v>
       </c>
       <c r="F219" s="14" t="s">
@@ -4962,15 +4972,15 @@
       </c>
     </row>
     <row r="220" spans="1:6">
-      <c r="A220" s="11"/>
-      <c r="B220" s="12"/>
-      <c r="C220" s="12">
+      <c r="A220" s="21"/>
+      <c r="B220" s="23"/>
+      <c r="C220" s="23">
         <v>7</v>
       </c>
       <c r="D220" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E220" s="15" t="s">
+      <c r="E220" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F220" s="14" t="s">
@@ -4978,208 +4988,208 @@
       </c>
     </row>
     <row r="221" spans="1:6">
-      <c r="A221" s="11"/>
-      <c r="B221" s="12"/>
-      <c r="C221" s="12">
+      <c r="A221" s="21"/>
+      <c r="B221" s="23"/>
+      <c r="C221" s="23">
         <v>8</v>
       </c>
       <c r="D221" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E221" s="15" t="s">
-        <v>73</v>
+      <c r="E221" s="24" t="s">
+        <v>214</v>
       </c>
       <c r="F221" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="222" spans="1:6">
-      <c r="A222" s="11"/>
-      <c r="B222" s="12"/>
-      <c r="C222" s="12">
+      <c r="A222" s="21"/>
+      <c r="B222" s="23"/>
+      <c r="C222" s="23">
         <v>9</v>
       </c>
       <c r="D222" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E222" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F222" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="21"/>
+      <c r="B223" s="23"/>
+      <c r="C223" s="23">
+        <v>10</v>
+      </c>
+      <c r="D223" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="E223" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F223" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="21"/>
+      <c r="B224" s="23"/>
+      <c r="C224" s="23">
+        <v>11</v>
+      </c>
+      <c r="D224" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E224" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F224" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225" s="21"/>
+      <c r="B225" s="23"/>
+      <c r="C225" s="23">
+        <v>12</v>
+      </c>
+      <c r="D225" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="E225" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F225" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="21"/>
+      <c r="B226" s="23"/>
+      <c r="C226" s="23">
+        <v>13</v>
+      </c>
+      <c r="D226" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E226" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F226" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="21"/>
+      <c r="B227" s="23"/>
+      <c r="C227" s="23">
+        <v>14</v>
+      </c>
+      <c r="D227" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E227" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F227" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="21"/>
+      <c r="B228" s="23"/>
+      <c r="C228" s="23">
+        <v>15</v>
+      </c>
+      <c r="D228" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E228" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="F228" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="21"/>
+      <c r="B229" s="23"/>
+      <c r="C229" s="23">
+        <v>16</v>
+      </c>
+      <c r="D229" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E229" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F229" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="21"/>
+      <c r="B230" s="23"/>
+      <c r="C230" s="23">
         <v>17</v>
       </c>
-      <c r="E222" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="F222" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223" s="11"/>
-      <c r="B223" s="12"/>
-      <c r="C223" s="12">
-        <v>10</v>
-      </c>
-      <c r="D223" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E223" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="F223" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="A224" s="11"/>
-      <c r="B224" s="12"/>
-      <c r="C224" s="12">
-        <v>11</v>
-      </c>
-      <c r="D224" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E224" s="15" t="s">
+      <c r="D230" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E230" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="F224" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6">
-      <c r="A225" s="11"/>
-      <c r="B225" s="12"/>
-      <c r="C225" s="12">
-        <v>12</v>
-      </c>
-      <c r="D225" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E225" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F225" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6">
-      <c r="A226" s="11"/>
-      <c r="B226" s="12"/>
-      <c r="C226" s="12">
-        <v>13</v>
-      </c>
-      <c r="D226" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="E226" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="F226" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6">
-      <c r="A227" s="11"/>
-      <c r="B227" s="12"/>
-      <c r="C227" s="12">
-        <v>14</v>
-      </c>
-      <c r="D227" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E227" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F227" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6">
-      <c r="A228" s="11"/>
-      <c r="B228" s="12"/>
-      <c r="C228" s="12">
-        <v>15</v>
-      </c>
-      <c r="D228" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E228" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F228" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6">
-      <c r="A229" s="11"/>
-      <c r="B229" s="12"/>
-      <c r="C229" s="12">
-        <v>16</v>
-      </c>
-      <c r="D229" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="E229" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="F229" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6">
-      <c r="A230" s="11"/>
-      <c r="B230" s="12"/>
-      <c r="C230" s="12">
-        <v>17</v>
-      </c>
-      <c r="D230" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="E230" s="15" t="s">
-        <v>222</v>
-      </c>
       <c r="F230" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="231" spans="1:6">
-      <c r="A231" s="11"/>
-      <c r="B231" s="12"/>
-      <c r="C231" s="12">
+      <c r="A231" s="21"/>
+      <c r="B231" s="23"/>
+      <c r="C231" s="23">
         <v>18</v>
       </c>
       <c r="D231" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="E231" s="15" t="s">
         <v>224</v>
       </c>
+      <c r="E231" s="24" t="s">
+        <v>225</v>
+      </c>
       <c r="F231" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="232" spans="1:6">
-      <c r="A232" s="11"/>
-      <c r="B232" s="12"/>
-      <c r="C232" s="12">
+      <c r="A232" s="21"/>
+      <c r="B232" s="23"/>
+      <c r="C232" s="23">
         <v>19</v>
       </c>
       <c r="D232" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="E232" s="15" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="E232" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F232" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="233" spans="1:6">
-      <c r="A233" s="11"/>
-      <c r="B233" s="12"/>
-      <c r="C233" s="12">
+      <c r="A233" s="21"/>
+      <c r="B233" s="23"/>
+      <c r="C233" s="23">
         <v>20</v>
       </c>
       <c r="D233" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="E233" s="15" t="s">
         <v>226</v>
+      </c>
+      <c r="E233" s="24" t="s">
+        <v>227</v>
       </c>
       <c r="F233" s="14" t="s">
         <v>8</v>
@@ -5188,30 +5198,26 @@
     <row r="234" spans="1:6">
       <c r="A234" s="11"/>
       <c r="B234" s="12"/>
-      <c r="C234" s="12">
-        <v>21</v>
-      </c>
-      <c r="D234" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E234" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F234" s="14" t="s">
-        <v>8</v>
-      </c>
+      <c r="C234" s="12"/>
+      <c r="D234" s="12"/>
+      <c r="E234" s="12"/>
+      <c r="F234" s="19"/>
     </row>
     <row r="235" spans="1:6">
-      <c r="A235" s="11"/>
-      <c r="B235" s="12"/>
+      <c r="A235" s="11">
+        <v>9</v>
+      </c>
+      <c r="B235" s="16" t="s">
+        <v>228</v>
+      </c>
       <c r="C235" s="12">
-        <v>22</v>
-      </c>
-      <c r="D235" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E235" s="15" t="s">
-        <v>192</v>
+        <v>1</v>
+      </c>
+      <c r="D235" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E235" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="F235" s="14" t="s">
         <v>8</v>
@@ -5220,26 +5226,30 @@
     <row r="236" spans="1:6">
       <c r="A236" s="11"/>
       <c r="B236" s="12"/>
-      <c r="C236" s="12"/>
-      <c r="D236" s="12"/>
-      <c r="E236" s="12"/>
-      <c r="F236" s="20"/>
+      <c r="C236" s="12">
+        <v>2</v>
+      </c>
+      <c r="D236" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E236" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F236" s="14" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="237" spans="1:6">
-      <c r="A237" s="11">
-        <v>9</v>
-      </c>
-      <c r="B237" s="16" t="s">
-        <v>227</v>
-      </c>
+      <c r="A237" s="11"/>
+      <c r="B237" s="12"/>
       <c r="C237" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D237" s="13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E237" s="12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F237" s="14" t="s">
         <v>8</v>
@@ -5249,13 +5259,13 @@
       <c r="A238" s="11"/>
       <c r="B238" s="12"/>
       <c r="C238" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D238" s="13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E238" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F238" s="14" t="s">
         <v>8</v>
@@ -5265,13 +5275,13 @@
       <c r="A239" s="11"/>
       <c r="B239" s="12"/>
       <c r="C239" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D239" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E239" s="12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F239" s="14" t="s">
         <v>8</v>
@@ -5281,13 +5291,13 @@
       <c r="A240" s="11"/>
       <c r="B240" s="12"/>
       <c r="C240" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D240" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E240" s="12" t="s">
-        <v>14</v>
+      <c r="E240" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="F240" s="14" t="s">
         <v>8</v>
@@ -5297,13 +5307,13 @@
       <c r="A241" s="11"/>
       <c r="B241" s="12"/>
       <c r="C241" s="12">
-        <v>5</v>
-      </c>
-      <c r="D241" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E241" s="12" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="D241" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E241" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="F241" s="14" t="s">
         <v>8</v>
@@ -5313,13 +5323,13 @@
       <c r="A242" s="11"/>
       <c r="B242" s="12"/>
       <c r="C242" s="12">
-        <v>6</v>
-      </c>
-      <c r="D242" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D242" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E242" s="15" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="F242" s="14" t="s">
         <v>8</v>
@@ -5329,13 +5339,13 @@
       <c r="A243" s="11"/>
       <c r="B243" s="12"/>
       <c r="C243" s="12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D243" s="18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E243" s="15" t="s">
-        <v>57</v>
+        <v>229</v>
       </c>
       <c r="F243" s="14" t="s">
         <v>8</v>
@@ -5345,13 +5355,13 @@
       <c r="A244" s="11"/>
       <c r="B244" s="12"/>
       <c r="C244" s="12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D244" s="18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E244" s="15" t="s">
-        <v>73</v>
+        <v>230</v>
       </c>
       <c r="F244" s="14" t="s">
         <v>8</v>
@@ -5361,13 +5371,13 @@
       <c r="A245" s="11"/>
       <c r="B245" s="12"/>
       <c r="C245" s="12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D245" s="18" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="E245" s="15" t="s">
-        <v>107</v>
+        <v>231</v>
       </c>
       <c r="F245" s="14" t="s">
         <v>8</v>
@@ -5377,13 +5387,13 @@
       <c r="A246" s="11"/>
       <c r="B246" s="12"/>
       <c r="C246" s="12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D246" s="18" t="s">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="E246" s="15" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="F246" s="14" t="s">
         <v>8</v>
@@ -5393,13 +5403,13 @@
       <c r="A247" s="11"/>
       <c r="B247" s="12"/>
       <c r="C247" s="12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D247" s="18" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E247" s="15" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F247" s="14" t="s">
         <v>8</v>
@@ -5409,13 +5419,13 @@
       <c r="A248" s="11"/>
       <c r="B248" s="12"/>
       <c r="C248" s="12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D248" s="18" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="E248" s="15" t="s">
-        <v>230</v>
+        <v>23</v>
       </c>
       <c r="F248" s="14" t="s">
         <v>8</v>
@@ -5425,13 +5435,13 @@
       <c r="A249" s="11"/>
       <c r="B249" s="12"/>
       <c r="C249" s="12">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D249" s="18" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
       <c r="E249" s="15" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F249" s="14" t="s">
         <v>8</v>
@@ -5441,13 +5451,13 @@
       <c r="A250" s="11"/>
       <c r="B250" s="12"/>
       <c r="C250" s="12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D250" s="18" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E250" s="15" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F250" s="14" t="s">
         <v>8</v>
@@ -5457,13 +5467,13 @@
       <c r="A251" s="11"/>
       <c r="B251" s="12"/>
       <c r="C251" s="12">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D251" s="18" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E251" s="15" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F251" s="14" t="s">
         <v>8</v>
@@ -5473,13 +5483,13 @@
       <c r="A252" s="11"/>
       <c r="B252" s="12"/>
       <c r="C252" s="12">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D252" s="18" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="E252" s="15" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F252" s="14" t="s">
         <v>8</v>
@@ -5489,13 +5499,13 @@
       <c r="A253" s="11"/>
       <c r="B253" s="12"/>
       <c r="C253" s="12">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D253" s="18" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E253" s="15" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="F253" s="14" t="s">
         <v>8</v>
@@ -5505,13 +5515,13 @@
       <c r="A254" s="11"/>
       <c r="B254" s="12"/>
       <c r="C254" s="12">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D254" s="18" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E254" s="15" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F254" s="14" t="s">
         <v>8</v>
@@ -5521,13 +5531,13 @@
       <c r="A255" s="11"/>
       <c r="B255" s="12"/>
       <c r="C255" s="12">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D255" s="18" t="s">
-        <v>235</v>
+        <v>106</v>
       </c>
       <c r="E255" s="15" t="s">
-        <v>238</v>
+        <v>107</v>
       </c>
       <c r="F255" s="14" t="s">
         <v>8</v>
@@ -5537,28 +5547,32 @@
       <c r="A256" s="11"/>
       <c r="B256" s="12"/>
       <c r="C256" s="12">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D256" s="18" t="s">
-        <v>235</v>
+        <v>106</v>
       </c>
       <c r="E256" s="15" t="s">
-        <v>239</v>
+        <v>192</v>
       </c>
       <c r="F256" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="257" spans="1:6">
-      <c r="A257" s="36"/>
-      <c r="F257" s="37"/>
+      <c r="A257" s="11"/>
+      <c r="B257" s="12"/>
+      <c r="C257" s="12"/>
+      <c r="D257" s="12"/>
+      <c r="E257" s="12"/>
+      <c r="F257" s="20"/>
     </row>
     <row r="258" spans="1:6">
-      <c r="A258" s="36">
+      <c r="A258" s="11">
         <v>10</v>
       </c>
-      <c r="B258" s="38" t="s">
-        <v>240</v>
+      <c r="B258" s="16" t="s">
+        <v>242</v>
       </c>
       <c r="C258" s="12">
         <v>1</v>
@@ -5574,7 +5588,8 @@
       </c>
     </row>
     <row r="259" spans="1:6">
-      <c r="A259" s="36"/>
+      <c r="A259" s="11"/>
+      <c r="B259" s="12"/>
       <c r="C259" s="12">
         <v>2</v>
       </c>
@@ -5589,7 +5604,8 @@
       </c>
     </row>
     <row r="260" spans="1:6">
-      <c r="A260" s="36"/>
+      <c r="A260" s="11"/>
+      <c r="B260" s="12"/>
       <c r="C260" s="12">
         <v>3</v>
       </c>
@@ -5604,7 +5620,8 @@
       </c>
     </row>
     <row r="261" spans="1:6">
-      <c r="A261" s="36"/>
+      <c r="A261" s="11"/>
+      <c r="B261" s="12"/>
       <c r="C261" s="12">
         <v>4</v>
       </c>
@@ -5619,7 +5636,8 @@
       </c>
     </row>
     <row r="262" spans="1:6">
-      <c r="A262" s="36"/>
+      <c r="A262" s="11"/>
+      <c r="B262" s="12"/>
       <c r="C262" s="12">
         <v>5</v>
       </c>
@@ -5627,14 +5645,15 @@
         <v>12</v>
       </c>
       <c r="E262" s="12" t="s">
-        <v>241</v>
+        <v>15</v>
       </c>
       <c r="F262" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="263" spans="1:6">
-      <c r="A263" s="36"/>
+      <c r="A263" s="11"/>
+      <c r="B263" s="12"/>
       <c r="C263" s="12">
         <v>6</v>
       </c>
@@ -5649,7 +5668,8 @@
       </c>
     </row>
     <row r="264" spans="1:6">
-      <c r="A264" s="36"/>
+      <c r="A264" s="11"/>
+      <c r="B264" s="12"/>
       <c r="C264" s="12">
         <v>7</v>
       </c>
@@ -5664,7 +5684,8 @@
       </c>
     </row>
     <row r="265" spans="1:6">
-      <c r="A265" s="36"/>
+      <c r="A265" s="11"/>
+      <c r="B265" s="12"/>
       <c r="C265" s="12">
         <v>8</v>
       </c>
@@ -5679,531 +5700,852 @@
       </c>
     </row>
     <row r="266" spans="1:6">
-      <c r="A266" s="36"/>
-      <c r="C266">
+      <c r="A266" s="11"/>
+      <c r="B266" s="12"/>
+      <c r="C266" s="12">
         <v>9</v>
       </c>
-      <c r="D266" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="E266" t="s">
+      <c r="D266" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E266" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F266" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6">
+      <c r="A267" s="11"/>
+      <c r="B267" s="12"/>
+      <c r="C267" s="12">
+        <v>10</v>
+      </c>
+      <c r="D267" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E267" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="F267" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6">
+      <c r="A268" s="11"/>
+      <c r="B268" s="12"/>
+      <c r="C268" s="12">
+        <v>11</v>
+      </c>
+      <c r="D268" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="F266" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6">
-      <c r="A267" s="36"/>
-      <c r="C267">
+      <c r="E268" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="F268" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6">
+      <c r="A269" s="11"/>
+      <c r="B269" s="12"/>
+      <c r="C269" s="12">
+        <v>12</v>
+      </c>
+      <c r="D269" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E269" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="F269" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6">
+      <c r="A270" s="11"/>
+      <c r="B270" s="12"/>
+      <c r="C270" s="12">
+        <v>13</v>
+      </c>
+      <c r="D270" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E270" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F270" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6">
+      <c r="A271" s="11"/>
+      <c r="B271" s="12"/>
+      <c r="C271" s="12">
+        <v>14</v>
+      </c>
+      <c r="D271" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E271" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F271" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
+      <c r="A272" s="11"/>
+      <c r="B272" s="12"/>
+      <c r="C272" s="12">
+        <v>15</v>
+      </c>
+      <c r="D272" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E272" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="F272" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6">
+      <c r="A273" s="11"/>
+      <c r="B273" s="12"/>
+      <c r="C273" s="12">
+        <v>16</v>
+      </c>
+      <c r="D273" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="E273" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="F273" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6">
+      <c r="A274" s="11"/>
+      <c r="B274" s="12"/>
+      <c r="C274" s="12">
+        <v>17</v>
+      </c>
+      <c r="D274" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E274" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F274" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6">
+      <c r="A275" s="11"/>
+      <c r="B275" s="12"/>
+      <c r="C275" s="12">
+        <v>18</v>
+      </c>
+      <c r="D275" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E275" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="F275" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6">
+      <c r="A276" s="11"/>
+      <c r="B276" s="12"/>
+      <c r="C276" s="12">
+        <v>19</v>
+      </c>
+      <c r="D276" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E276" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="F276" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6">
+      <c r="A277" s="11"/>
+      <c r="B277" s="12"/>
+      <c r="C277" s="12">
+        <v>20</v>
+      </c>
+      <c r="D277" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E277" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="F277" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6">
+      <c r="A278" s="11"/>
+      <c r="F278" s="20"/>
+    </row>
+    <row r="279" spans="1:6">
+      <c r="A279" s="11">
+        <v>11</v>
+      </c>
+      <c r="B279" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="C279" s="12">
+        <v>1</v>
+      </c>
+      <c r="D279" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E279" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F279" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6">
+      <c r="A280" s="11"/>
+      <c r="C280" s="12">
+        <v>2</v>
+      </c>
+      <c r="D280" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E280" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F280" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6">
+      <c r="A281" s="11"/>
+      <c r="C281" s="12">
+        <v>3</v>
+      </c>
+      <c r="D281" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E281" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F281" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6">
+      <c r="A282" s="11"/>
+      <c r="C282" s="12">
+        <v>4</v>
+      </c>
+      <c r="D282" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E282" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F282" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6">
+      <c r="A283" s="11"/>
+      <c r="C283" s="12">
+        <v>5</v>
+      </c>
+      <c r="D283" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E283" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F283" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6">
+      <c r="A284" s="11"/>
+      <c r="C284" s="12">
+        <v>6</v>
+      </c>
+      <c r="D284" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E284" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F284" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6">
+      <c r="A285" s="11"/>
+      <c r="C285" s="12">
+        <v>7</v>
+      </c>
+      <c r="D285" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E285" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F285" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6">
+      <c r="A286" s="11"/>
+      <c r="C286" s="12">
+        <v>8</v>
+      </c>
+      <c r="D286" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E286" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F286" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6">
+      <c r="A287" s="11"/>
+      <c r="C287">
+        <v>9</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E287" t="s">
+        <v>258</v>
+      </c>
+      <c r="F287" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6">
+      <c r="A288" s="11"/>
+      <c r="C288">
         <v>10</v>
       </c>
-      <c r="D267" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="E267" t="s">
-        <v>244</v>
-      </c>
-      <c r="F267" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6">
-      <c r="A268" s="36"/>
-      <c r="C268">
+      <c r="D288" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E288" t="s">
+        <v>259</v>
+      </c>
+      <c r="F288" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6">
+      <c r="A289" s="11"/>
+      <c r="C289">
         <v>11</v>
       </c>
-      <c r="D268" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="E268" t="s">
-        <v>245</v>
-      </c>
-      <c r="F268" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6">
-      <c r="A269" s="36"/>
-      <c r="C269">
-        <v>12</v>
-      </c>
-      <c r="D269" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="E269" t="s">
-        <v>247</v>
-      </c>
-      <c r="F269" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6">
-      <c r="A270" s="36"/>
-      <c r="C270" s="22">
+      <c r="D289" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E289" t="s">
+        <v>260</v>
+      </c>
+      <c r="F289" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6">
+      <c r="A290" s="11"/>
+      <c r="C290">
+        <v>12</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E290" t="s">
+        <v>262</v>
+      </c>
+      <c r="F290" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6">
+      <c r="A291" s="11"/>
+      <c r="C291" s="12">
         <v>16</v>
       </c>
-      <c r="D270" s="30" t="s">
+      <c r="D291" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E270" s="22" t="s">
+      <c r="E291" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F270" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6">
-      <c r="A271" s="36"/>
-      <c r="C271" s="22">
+      <c r="F291" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6">
+      <c r="A292" s="11"/>
+      <c r="C292" s="12">
         <v>17</v>
       </c>
-      <c r="D271" s="30" t="s">
+      <c r="D292" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E271" s="22" t="s">
+      <c r="E292" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="F271" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6">
-      <c r="A272" s="36"/>
-      <c r="C272" s="22">
+      <c r="F292" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6">
+      <c r="A293" s="11"/>
+      <c r="C293" s="12">
         <v>18</v>
       </c>
-      <c r="D272" s="30" t="s">
+      <c r="D293" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E272" s="22" t="s">
+      <c r="E293" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="F272" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6">
-      <c r="A273" s="36"/>
-      <c r="C273">
+      <c r="F293" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6">
+      <c r="A294" s="11"/>
+      <c r="C294">
         <v>19</v>
       </c>
-      <c r="D273" s="30" t="s">
+      <c r="D294" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E273" t="s">
-        <v>248</v>
-      </c>
-      <c r="F273" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6">
-      <c r="A274" s="36"/>
-      <c r="F274" s="37"/>
-    </row>
-    <row r="275" spans="1:6">
-      <c r="A275" s="36">
+      <c r="E294" t="s">
+        <v>263</v>
+      </c>
+      <c r="F294" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6">
+      <c r="A295" s="11"/>
+      <c r="F295" s="20"/>
+    </row>
+    <row r="296" spans="1:6">
+      <c r="A296" s="11">
+        <v>12</v>
+      </c>
+      <c r="B296" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="C296" s="12">
+        <v>1</v>
+      </c>
+      <c r="D296" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E296" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F296" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6">
+      <c r="A297" s="11"/>
+      <c r="C297" s="12">
+        <v>2</v>
+      </c>
+      <c r="D297" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E297" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F297" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6">
+      <c r="A298" s="11"/>
+      <c r="C298" s="12">
+        <v>3</v>
+      </c>
+      <c r="D298" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E298" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F298" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6">
+      <c r="A299" s="11"/>
+      <c r="C299" s="12">
+        <v>4</v>
+      </c>
+      <c r="D299" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E299" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F299" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6">
+      <c r="A300" s="11"/>
+      <c r="C300" s="12">
+        <v>5</v>
+      </c>
+      <c r="D300" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E300" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="F300" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6">
+      <c r="A301" s="11"/>
+      <c r="C301" s="12">
+        <v>6</v>
+      </c>
+      <c r="D301" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E301" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F301" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6">
+      <c r="A302" s="11"/>
+      <c r="C302" s="12">
+        <v>7</v>
+      </c>
+      <c r="D302" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E302" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F302" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6">
+      <c r="A303" s="11"/>
+      <c r="C303" s="12">
+        <v>8</v>
+      </c>
+      <c r="D303" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E303" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F303" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6">
+      <c r="A304" s="11"/>
+      <c r="C304">
+        <v>9</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E304" t="s">
+        <v>266</v>
+      </c>
+      <c r="F304" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6">
+      <c r="A305" s="11"/>
+      <c r="C305">
+        <v>10</v>
+      </c>
+      <c r="D305" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E305" t="s">
+        <v>267</v>
+      </c>
+      <c r="F305" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6">
+      <c r="A306" s="11"/>
+      <c r="C306">
+        <v>12</v>
+      </c>
+      <c r="D306" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E306" t="s">
+        <v>269</v>
+      </c>
+      <c r="F306" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6">
+      <c r="A307" s="11"/>
+      <c r="F307" s="20"/>
+    </row>
+    <row r="308" spans="1:6">
+      <c r="A308" s="11">
+        <v>13</v>
+      </c>
+      <c r="B308" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="C308">
+        <v>1</v>
+      </c>
+      <c r="D308" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E308" t="s">
+        <v>272</v>
+      </c>
+      <c r="F308" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6">
+      <c r="A309" s="11"/>
+      <c r="C309">
+        <v>2</v>
+      </c>
+      <c r="D309" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E309" t="s">
+        <v>273</v>
+      </c>
+      <c r="F309" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6">
+      <c r="A310" s="11"/>
+      <c r="C310">
+        <v>3</v>
+      </c>
+      <c r="D310" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E310" t="s">
+        <v>274</v>
+      </c>
+      <c r="F310" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6">
+      <c r="A311" s="11"/>
+      <c r="C311">
+        <v>4</v>
+      </c>
+      <c r="D311" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E311" t="s">
+        <v>276</v>
+      </c>
+      <c r="F311" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6">
+      <c r="A312" s="11"/>
+      <c r="C312">
+        <v>5</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E312" t="s">
+        <v>277</v>
+      </c>
+      <c r="F312" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6">
+      <c r="A313" s="11"/>
+      <c r="C313">
+        <v>6</v>
+      </c>
+      <c r="D313" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E313" t="s">
+        <v>279</v>
+      </c>
+      <c r="F313" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6">
+      <c r="A314" s="11"/>
+      <c r="C314">
+        <v>7</v>
+      </c>
+      <c r="D314" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E314" t="s">
+        <v>280</v>
+      </c>
+      <c r="F314" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6">
+      <c r="A315" s="11"/>
+      <c r="C315">
+        <v>8</v>
+      </c>
+      <c r="D315" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E315" t="s">
+        <v>282</v>
+      </c>
+      <c r="F315" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6">
+      <c r="A316" s="11"/>
+      <c r="C316">
+        <v>9</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E316" t="s">
+        <v>283</v>
+      </c>
+      <c r="F316" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6">
+      <c r="A317" s="11"/>
+      <c r="C317">
+        <v>10</v>
+      </c>
+      <c r="D317" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E317" t="s">
+        <v>284</v>
+      </c>
+      <c r="F317" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6">
+      <c r="A318" s="11"/>
+      <c r="C318">
         <v>11</v>
       </c>
-      <c r="B275" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="C275" s="12">
-        <v>1</v>
-      </c>
-      <c r="D275" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E275" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F275" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6">
-      <c r="A276" s="36"/>
-      <c r="C276" s="12">
-        <v>2</v>
-      </c>
-      <c r="D276" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E276" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F276" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6">
-      <c r="A277" s="36"/>
-      <c r="C277" s="12">
-        <v>3</v>
-      </c>
-      <c r="D277" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E277" s="12" t="s">
+      <c r="D318" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E318" t="s">
+        <v>282</v>
+      </c>
+      <c r="F318" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6">
+      <c r="A319" s="11"/>
+      <c r="C319">
+        <v>12</v>
+      </c>
+      <c r="D319" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E319" t="s">
+        <v>283</v>
+      </c>
+      <c r="F319" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6">
+      <c r="A320" s="11"/>
+      <c r="C320">
         <v>13</v>
       </c>
-      <c r="F277" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6">
-      <c r="A278" s="36"/>
-      <c r="C278" s="12">
-        <v>4</v>
-      </c>
-      <c r="D278" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E278" s="12" t="s">
+      <c r="D320" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E320" t="s">
+        <v>286</v>
+      </c>
+      <c r="F320" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6">
+      <c r="A321" s="26"/>
+      <c r="B321" s="27"/>
+      <c r="C321" s="27">
         <v>14</v>
       </c>
-      <c r="F278" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6">
-      <c r="A279" s="36"/>
-      <c r="C279" s="12">
-        <v>5</v>
-      </c>
-      <c r="D279" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E279" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="F279" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6">
-      <c r="A280" s="36"/>
-      <c r="C280" s="12">
-        <v>6</v>
-      </c>
-      <c r="D280" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E280" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F280" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6">
-      <c r="A281" s="36"/>
-      <c r="C281" s="12">
-        <v>7</v>
-      </c>
-      <c r="D281" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E281" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F281" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6">
-      <c r="A282" s="36"/>
-      <c r="C282" s="12">
-        <v>8</v>
-      </c>
-      <c r="D282" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E282" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F282" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6">
-      <c r="A283" s="36"/>
-      <c r="C283">
-        <v>9</v>
-      </c>
-      <c r="D283" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="E283" t="s">
-        <v>251</v>
-      </c>
-      <c r="F283" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6">
-      <c r="A284" s="36"/>
-      <c r="C284">
-        <v>10</v>
-      </c>
-      <c r="D284" s="39" t="s">
-        <v>250</v>
-      </c>
-      <c r="E284" t="s">
-        <v>252</v>
-      </c>
-      <c r="F284" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6">
-      <c r="A285" s="36"/>
-      <c r="C285">
-        <v>12</v>
-      </c>
-      <c r="D285" s="39" t="s">
-        <v>253</v>
-      </c>
-      <c r="E285" t="s">
-        <v>254</v>
-      </c>
-      <c r="F285" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6">
-      <c r="A286" s="36"/>
-      <c r="F286" s="37"/>
-    </row>
-    <row r="287" spans="1:6">
-      <c r="A287" s="36">
-        <v>12</v>
-      </c>
-      <c r="B287" s="38" t="s">
-        <v>255</v>
-      </c>
-      <c r="C287">
-        <v>1</v>
-      </c>
-      <c r="D287" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="E287" t="s">
-        <v>257</v>
-      </c>
-      <c r="F287" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6">
-      <c r="A288" s="36"/>
-      <c r="C288">
-        <v>2</v>
-      </c>
-      <c r="D288" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="E288" t="s">
-        <v>258</v>
-      </c>
-      <c r="F288" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6">
-      <c r="A289" s="36"/>
-      <c r="C289">
-        <v>3</v>
-      </c>
-      <c r="D289" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="E289" t="s">
-        <v>259</v>
-      </c>
-      <c r="F289" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6">
-      <c r="A290" s="36"/>
-      <c r="C290">
-        <v>4</v>
-      </c>
-      <c r="D290" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="E290" t="s">
-        <v>261</v>
-      </c>
-      <c r="F290" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6">
-      <c r="A291" s="36"/>
-      <c r="C291">
-        <v>5</v>
-      </c>
-      <c r="D291" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="E291" t="s">
-        <v>262</v>
-      </c>
-      <c r="F291" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6">
-      <c r="A292" s="36"/>
-      <c r="C292">
-        <v>6</v>
-      </c>
-      <c r="D292" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="E292" t="s">
-        <v>264</v>
-      </c>
-      <c r="F292" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6">
-      <c r="A293" s="36"/>
-      <c r="C293">
-        <v>7</v>
-      </c>
-      <c r="D293" s="39" t="s">
-        <v>263</v>
-      </c>
-      <c r="E293" t="s">
-        <v>265</v>
-      </c>
-      <c r="F293" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6">
-      <c r="A294" s="36"/>
-      <c r="C294">
-        <v>8</v>
-      </c>
-      <c r="D294" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="E294" t="s">
-        <v>267</v>
-      </c>
-      <c r="F294" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6">
-      <c r="A295" s="36"/>
-      <c r="C295">
-        <v>9</v>
-      </c>
-      <c r="D295" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="E295" t="s">
-        <v>268</v>
-      </c>
-      <c r="F295" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6">
-      <c r="A296" s="36"/>
-      <c r="C296">
-        <v>10</v>
-      </c>
-      <c r="D296" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="E296" t="s">
-        <v>269</v>
-      </c>
-      <c r="F296" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6">
-      <c r="A297" s="36"/>
-      <c r="C297">
-        <v>11</v>
-      </c>
-      <c r="D297" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="E297" t="s">
-        <v>267</v>
-      </c>
-      <c r="F297" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="298" spans="1:6">
-      <c r="A298" s="36"/>
-      <c r="C298">
-        <v>12</v>
-      </c>
-      <c r="D298" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="E298" t="s">
-        <v>268</v>
-      </c>
-      <c r="F298" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6">
-      <c r="A299" s="36"/>
-      <c r="C299">
-        <v>13</v>
-      </c>
-      <c r="D299" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="E299" t="s">
-        <v>271</v>
-      </c>
-      <c r="F299" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6">
-      <c r="A300" s="40"/>
-      <c r="B300" s="41"/>
-      <c r="C300" s="41">
-        <v>14</v>
-      </c>
-      <c r="D300" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="E300" s="41" t="s">
-        <v>273</v>
-      </c>
-      <c r="F300" s="43" t="s">
+      <c r="D321" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="E321" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F321" s="29" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F144:F190 F4:F142 F258:F273 F275:F285 F287:F300">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 F144:F189 F4:F142 F214:F233">
       <formula1>$AA$2:$AA$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F143">
       <formula1>$H$2:$H$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F191:F235 F237:F256">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F279:F294 F308:F321 F258:F277 F296:F306 F234:F256 F190:F213">
       <formula1>$AA$2:$AA$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F257 F236 F286">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F278 F257 F307">
       <formula1>$H$2:$H$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>